<commit_message>
tipo de descripciones de cada fuente técnicas o claras
</commit_message>
<xml_diff>
--- a/Datos/Datos VertebradosIbericos/Descripciones Aves.xlsx
+++ b/Datos/Datos VertebradosIbericos/Descripciones Aves.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hackaton_Biodiversidad_IA_2025\Hackathon-PNAV\Datos\Datos VertebradosIbericos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B2690D-C5B9-4AE1-917A-8B00978D6424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBDF22C-9F7A-405D-8887-D328AD32E6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="386">
   <si>
     <t>Commun Name</t>
   </si>
@@ -66,21 +66,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Merops apiaster</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color rgb="FFC0C0C0"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t> Linnaeus, 1758</t>
-    </r>
-  </si>
-  <si>
     <t>Merops apiaster Linnaeus, 1758</t>
   </si>
   <si>
@@ -803,12 +788,669 @@
     <t>Paseriforme de tamaño mediano (21-23 cm). El macho adulto es de color negro lustroso, con tonalidades irisadas. Las hembras adultas presentan libreas que van del negro a un pardo muy oscuro, con un lustre muy variable. Los jóvenes antes de su primera muda son de color pardo uniforme. Después de su primera muda adquieren el plumaje adulto, pero presentan motas blancas, más conspicuas en las hembras.
 Masa corporal media, 91 g en machos y 86 g en hembras.</t>
   </si>
+  <si>
+    <t>Flamenco común</t>
+  </si>
+  <si>
+    <t>Phoenicopterus roseus Pallas, 1811</t>
+  </si>
+  <si>
+    <t>Cuello y patas alargados, pico curvo y alas largas y estrechas. Pico rosado con la punta negra, patas rojizas e iris amarillo en adultos. Plumaje rosa pálido en adultos, similar en ambos sexos, con moteado salmón o carmesí en las coberteras superiores e inferiores de las alas. Las primarias y secundarias son de color negro. La intensidad de la coloración rosada puede variar estacionalmente por la aplicación de carotenoides, a modo de maquillaje, desde la glándula uropigial a las plumas.
+Los pollos recién nacidos tienen plumón blanquecino que se torna progresivamente grisáceo hasta que a los 10 días de vida es completamente gris oscuro. Entre los 3-5 meses de edad, los juveniles son de color gris-marrón. Los pollos volantones presentan plumaje más blanquecino en las coberteras superiores, cuello y cabeza. Entre 1 y 2 años de edad, las coberteras inferiores son marrones con partes blancas y rosa intercaladas. Hay algunas plumas grisáceas en cuello y coberteras superiores. Entre 2-3 años de edad el plumaje es muy similar al de los adultos, aunque pueden presentar color marrón en la base de las plumas coberteras superiores.
+Longitud total, 120-145 cm; envergadura, 140-187 cm; masa corporal media, 2,9 kg en machos y 2,5 kg en hembras.</t>
+  </si>
+  <si>
+    <t>Focha moruna</t>
+  </si>
+  <si>
+    <r>
+      <t>Fulica cristata</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFC0C0C0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> J. F. Gmelin, 1789</t>
+    </r>
+  </si>
+  <si>
+    <t>Ave tímida de tamaño mediano muy parecida a la focha común Fulica atra, con un aspecto muy similar en machos y hembras- No obstante, el tamaño de los machos supera en general un 5% al de las hembras. Tiene el plumaje oscuro con algunos reflejos verdosos. Cuenta con un escudete frontal blanco, un pico de tono celeste pálido y unas protuberancias rojas a ambos lados del escudete frontal más conspicuas en animales adultos y sobre todo en época de celo. El pie suele ser de un color verde oscuro que pasa a ser de color azul grisáceo fuera del periodo de reproducción.
+Los individuos jóvenes también son similares a los de focha común, aunque los de focha moruna son mucho más oscuros. En los jóvenes las protuberancias rojas están menos desarrolladas y los polluelos carecen de ellas, así como de plumaje a los lados de la cabeza.
+El peso medio del macho es de 0,840 kg mientras que el peso medio de la hembra es de 0,623 kg.</t>
+  </si>
+  <si>
+    <t>Ganga ibérica</t>
+  </si>
+  <si>
+    <r>
+      <t> Pterocles alchata</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFC0C0C0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> (Linnaeus, 1766)</t>
+    </r>
+  </si>
+  <si>
+    <t>Tamaño similar al de una paloma, con patas cortas y un cuerpo rechoncho de aspecto críptico y dorso de color terroso. El vientre y la cara inferior de las alas son de color blanco, mientras que las partes superiores presentan un color pardusco general y manchas de colores que difieren entre sexos (amarillas en machos y gris azuladas en hembras). La cola es larga y afilada. En el pecho, banda ancha de color castaño flanqueada con líneas negras. Pico corto de color gris azulado y anillo orbital de color azul. Alas largas y apuntadas que permiten un vuelo directo y rápido. Juveniles con aspecto parecido al de las hembras pero con colores más apagados, sin motas gris azulado en el dorso y cola corta; lista ocular de color blanquecino característica.
+Masa corporal media, 348 g en machos y 319 g en hembras.</t>
+  </si>
+  <si>
+    <t>Garceta común</t>
+  </si>
+  <si>
+    <r>
+      <t>Egretta garzetta</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFC0C0C0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> (Linnaeus, 1766)</t>
+    </r>
+  </si>
+  <si>
+    <t>Garza de tamaño medio (55-65 cm de longitud) con plumaje enteramente blanco, pico negro y patas también negras, excepto los pies, que en la subespecie nominal son amarillos. Tiene también amarillo el iris y su lorum es azulado-grisáceo. En periodo reproductor los adultos exhiben dos características plumas lanceoladas en la coronilla, que pueden alcanzar los 16 cm, y también plumas ornamentales largas en el pecho y la espalda. Los dedos y el lorum se tornan anaranjados durante el apogeo del cortejo. Los jóvenes son parecidos a los adultos pero no tienen plumas alargadas, sus patas son negro-verdosas y, en la subespecie nominal, los pies son de un amarillo menos intenso.
+Masa corporal, entre 450-614 g en machos y 490-530 g en hembras.</t>
+  </si>
+  <si>
+    <t>Gaviota cabecinegra</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ichthyaetus melanocephalus (Temminck, 1820)</t>
+  </si>
+  <si>
+    <t>Adulto con cabeza negra, más extenso que en la gaviota reidora, se interna sobradamente en la parte superior del cuello. El pico y las patas son rojo coral. Con una franja negra en el extremo del pico y punta clara. Plumaje gris muy claro en partes superiores y blanco en el cuello y partes inferiores. En invierno, la cabeza y el cuello, blanquecinos, ambos tonos uniformes. Longitud entre 37 y 40 cm y envergadura de entre 94 y 102 cm.
+Masa corporal media, 288 g en machos y 257 g en hembras.</t>
+  </si>
+  <si>
+    <t>Gaviota patiamarilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Larus michahellis Naumann, 1840</t>
+  </si>
+  <si>
+    <t>Gaviota perteneciente al grupo de los grandes láridos con cabeza blanca (en época de cría), con cuatro grupos de edad. Los plumajes de primer a tercer año presentan, progresivamente, cada vez menos pardo y más gris en zona dorsal y alas. Los adultos son blancos, con el manto y parte superior de las alas de un gris más oscuro que la argéntea L. argentatus pero más claro que la sombría L. fuscus. Acusado dimorfismo sexual en tamaño y peso, siendo los machos más grandes y pesados. Existe, además, amplia variación regional.</t>
+  </si>
+  <si>
+    <t>Gorrión alpino</t>
+  </si>
+  <si>
+    <t>Montifringilla nivalis (Linnaeus, 1766)</t>
+  </si>
+  <si>
+    <t>17-17,5 cm; ave con aspecto de fringílido y largas colas y alas, de pico fuerte y puntiagudo. Cabeza y cogote gris azulado, mentón y garganta negros, partes superiores pardo chocolate, obispillo y supracobertoras caudales negras, y alas que muestran gran panel blanco en vuelo. Pico y patas negras. Hembra similar al macho pero algo más pardusca y babero menos definido.
+Masa corporal, 31-57 g.</t>
+  </si>
+  <si>
+    <t>Gorrión común</t>
+  </si>
+  <si>
+    <t>Passer domesticus (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Ave de pequeño tamaño pero robusta, de cabeza comparativamente grande y de pico bien desarrollado. Muestra colores pardos muy poco contrastados en las hembras o juveniles y mucho más marcados en los machos. Puede confundirse con el Gorrión moruno Passer hispanoliensis o con el Gorrión molinero Passer montanus o con híbridos de estas especies. El macho de Gorrión común posee un diseño de plumaje en la cabeza claramente diferenciado de las otras dos especies, mostrando un píleo de color gris. Sin embargo, las hembras o los juveniles de Gorrión común y de Gorrión moruno pueden ser indistinguibles visualmente.
+El macho muestra una frente y píleo de color gris oliváceo. Bridas estrechas de color negro que forman una corta región malar también de color negro. Estrecha y corta lista ocular de color negro en su base y blanco en la parte superior. Ceja ancha de color pardo claro que se extiende hasta la nuca y la parte superior del cuello. Auriculares de color gris oliváceo sucio que se aclaran progresivamente, mostrando un aspecto gris blanquecino en las mejillas. Mentón y garganta de color negro formando un babero.
+Dorso y escapulares de color castaño oscuro. Espalda, obispillo y supracobertoras caudales de color gris oliváceo. El pecho, los flancos y los muslos presentan un color grisáceo claro. La cola de color pardo amarillento. 
+Hembra con la frente y el píleo de color pardo oscuro con un tinte oliváceo que se transforma en un pardo más claro en la nuca y la parte superior del cuello. Posee una ceja bien marcada de color pardo amarillento o canela, que se extiende desde el ojo hasta casi la nuca, y que queda limitada por debajo por una estrecha lista ocular de color negro apagado. Auriculares y mejillas de color marrón oliváceo. Mentón y garganta de color pardo grisáceo, que puede albergar pequeñas manchas de color gris oscuro formando un pequeño e irregular babero. Dorso y escapulares de color canela estriados de negro. La espalda, el obispillo y las supracobertoras caudales son de un color castaño oliváceo. El plumaje de las alas es de color canela sucio.
+Masa corporal media, 27,6 g.</t>
+  </si>
+  <si>
+    <t>Gorrión molinero</t>
+  </si>
+  <si>
+    <t>Passer montanus (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Pequeño pájaro de 14 cm de longitud y 22 cm de envergadura. Sin dimorfismo sexual. Plumaje de tonos pardos con rayas negras en el dorso y gris pálido en la parte inferior. Presenta una característica mancha negra en cada una de las mejillas. Más pequeño y de aspecto más rechoncho y delicado que otros gorriones.
+Masa corporal media, 19,8 g.</t>
+  </si>
+  <si>
+    <t>Gorrión moruno</t>
+  </si>
+  <si>
+    <t>Passer hispaniolensis (Temminck, 1820)</t>
+  </si>
+  <si>
+    <t>Ave de 14 cm de longitud. Macho con dorso pardo con listas negras densas. Píleo y cogote castaños, partes inferiores y mejillas blancas, babero negro que se extiende por el pecho y a lo largo de los flancos en líneas. Hembra y joven blanco sucio por debajo y pardo con listas más oscuras por arriba y algunas listas tenues en pecho y flancos.
+Masa corporal media: 28 g.</t>
+  </si>
+  <si>
+    <t>Graja</t>
+  </si>
+  <si>
+    <t>Corvus frugilegus Linnaeus, 1758</t>
+  </si>
+  <si>
+    <t>Córvido un poco menor que la corneja negra (Corvus corone), con pico más fino, menor cabeza con frente más alta y apariencia de cuerpo grande que se debe a las plumas del flanco y calzas; al volar muestra las puntas de las alas bien digitadas y una cola mas redonda. Aspecto elegante en el que destacan las partes calvas de cara y base del pico propias de los adultos y, siempre, las calzas de pluma sueltas sobre las patas. El plumaje negro es muy brillante. Los sexos son iguales. Los juveniles carecen de las zonas peladas y se parecen a las cornejas negras.
+Son también caracteres diferenciales con la corneja su tendencia a volar en grupos, a realizar vuelos acrobáticos al estilo de las chovas y su reclamo.
+Masa corporal media, 469,8 g en machos y 401,5 g en hembras.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grajilla </t>
+  </si>
+  <si>
+    <t>Corvus monedula Linnaeus, 1758</t>
+  </si>
+  <si>
+    <t>Córvido de pequeño tamaño (33 cm) y de color negro. El carácter más distintivo es la presencia de una zona gris pálida en los laterales de la cabeza (detrás del ojo) y nuca.
+Masa corporal media: machos, 230 g; hembras, 206 g.</t>
+  </si>
+  <si>
+    <t>Grulla común</t>
+  </si>
+  <si>
+    <t>Grus grus (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Ave de color grisáceo y tamaño grande (110 cm de longitud y 200 cm de envergadura). Aspecto esbelto con patas y cuello alargados. Cabeza con píleo rojo enmarcado en una franja negra anterior y posterior y que cubre la garganta y la mitad superior del cuello. Franjas blancas desde las mejillas hasta que se unen en la parte media trasera del cuello. Cola corta. Las plumas primarias y secundarias de las alas son negras. La coloración de la cabeza en los jóvenes es parda.
+Masa corporal media, 5,7 kg.</t>
+  </si>
+  <si>
+    <t>Halcón peregrino</t>
+  </si>
+  <si>
+    <t>Falco peregrinus Tunstall, 1771</t>
+  </si>
+  <si>
+    <t>Dorso entre gris-azulado y negro, vientre entre blanco y ocre, casco negro con una bigotera marcada y mejilla blanca.
+Masa corporal: macho, 540-637 g; hembra, 775-970 g.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herrerillo común </t>
+  </si>
+  <si>
+    <t>Cyanistes caeruleus (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dorso verde pardo y vientre amarillo con pequeña banda vertical negra. Alas y cola azules. Mejillas y parte superior de la cabeza blancas, con mancha azul en la parte superior. Banda oscura desde al pico a la nuca pasando por el ojo.
+</t>
+  </si>
+  <si>
+    <t>Herrerillo africano</t>
+  </si>
+  <si>
+    <t>Cyanistes teneriffae (Lesson, 1831)</t>
+  </si>
+  <si>
+    <t>Dorso verde pardo y vientre amarillo, excepto en La Palma que es blancuzco. Alas y cola azules. Mejillas y parte superior de la cabeza blancas, con mancha azul en la parte superior. Banda oscura desde al pico a la nuca pasando por el ojo. Hay leve variación de la coloración entre islas.
+Masa corporal, 9-12 g.</t>
+  </si>
+  <si>
+    <t>Herrerillo capuchino</t>
+  </si>
+  <si>
+    <t>Lophophanes cristatus (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Paseriforme de pequeño tamaño (11,5 cm). Fácilmente distinguible por la cresta de color negra y blanca. La parte ventral color ante, mientras que la dorsal, incluyendo alas y cola, de color pardo. Destaca una garganta negra que se extiende hacia atrás creando una especie de collar, paralelamente otro de color blanco. El macho y la hembra son del mismo color y tamaño. Los adultos, con iris rojizo, se diferencian de los individuos de primer año al realizar estos últimos solo una muda parcial. Los juveniles tienen el iris pardo.
+Masa corporal media, 11,6 g.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ibis eremita </t>
+  </si>
+  <si>
+    <t>Geronticus eremita (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>El ibis eremita es un ibis de tamaño mediano y, a diferencia de otras especies de ibis, no presenta largas patas y cuello, lo que le confiere un aspecto menos estilizado. El plumaje del adulto es verde metálico oscuro o negro brillante, con iridiscencias de color violeta y una mancha cobriza en las rémiges y coberteras secundarias. Tiene la cabeza desnuda y la piel expuesta es de color rojizo con patrones variables de manchas oscuras, coronada con un penacho de plumas. Tiene patas rojizas, y un pico largo curvado hacia abajo de color rojizo. En ambos sexos las partes desnudas de plumas son más brillantes durante la época de reproducción. No existe dimorfismo sexual acusado. Los juveniles de primer año son más apagados, menos brillantes, con plumaje negro mate que carece de la mancha cobriza en las alas. La cabeza está completamente cubierta de plumas y el iris es de color grisáceo. A medida que las aves maduran se va coloreando de anaranjado hasta ser casi amarillento en los adultos. En el segundo año van perdiendo parte de las plumas de la cabeza, pudiendo quedar algunas sueltas en cara o garganta, adquieren brillo violeta en las coberteras de las alas y evidencia de cresta nucal. En su tercer año, la cabeza y garganta quedan desprovistas de plumas, quedando “calvos” con un penacho de largas plumas en nuca. En campo, el aspecto del ibis eremita sólo podría confundirse con el otro ibis ibérico: el morito común (Plegadis falcinelus), de menor talla, aspecto más grácil y cabeza siempre emplumada.  En vuelo, las patas del ibis eremita no sobrepasan la longitud de la cola mientras que en el morito son proporcionalmente más largas y cuelgan hacia atrás sobrepasando el nivel de la cola.</t>
+  </si>
+  <si>
+    <t>Lagópodo alpino</t>
+  </si>
+  <si>
+    <t>Lagopus muta (Montin, 1776)</t>
+  </si>
+  <si>
+    <t>Ave de pequeñas dimensiones, mide entre 34-36 cm de largo, con una envergadura alar de 54-60 cm. Presentan patas completamente recubiertas de plumas, incluso la porción distal de los dedos, quedando solo descubiertas las uñas, de esta forma poseen un mayor aislamiento térmico y reducen el gasto energético al caminar sobre la nieve.
+Poseen un pico negro y corto y una carúncula o carnosidad roja por encima de los ojos (mayor en los machos) y una estría negra desde el pico hasta los ojos (los machos).
+En la época estival son de tonalidades grises, conservando la parte inferior de las alas y vientre blancos. En invierno adquiere su característico color blanco uniforme, a excepción de la cola negra. Los jóvenes son similares a los adultos, tanto en verano, como en invierno.
+Masa corporal media, 466 g en machos y 429 g en hembras.</t>
+  </si>
+  <si>
+    <t>Lavandera boyera</t>
+  </si>
+  <si>
+    <t>Motacilla flava Linnaeus, 1758</t>
+  </si>
+  <si>
+    <t>Pájaro de 15-16 cm de longitud, aspecto general estilizado, y con plumaje esencialmente similar en ambos sexos, aunque bastante más intensamente coloreado en los machos, especialmente en periodo reproductor. El pecho, vientre y zona anal son de color amarillo, mientras que el manto, el dorso y el obispillo son de color pardo oliváceo. Las alas son grisáceas, y las patas y el pico son negros.
+Masa corporal media, 21 g.</t>
+  </si>
+  <si>
+    <t>Lavandera cascadeña </t>
+  </si>
+  <si>
+    <t>Motacilla cinerea Tunstall, 1771</t>
+  </si>
+  <si>
+    <t>Pájaro de 17-20 cm de longitud, estilizado, de cola larga con plumas centrales negras y externas blancas, muy característica. Plumaje general grisáceo oscuro en el dorso con el obispillo y partes inferiores amarillentas (pecho, vientre), más brillantes en la zona anal. Esencialmente parecidos en ambos sexos aunque más intensamente contrastado en los machos que, durante el periodo reproductor, exhiben un característico babero negro.</t>
+  </si>
+  <si>
+    <t>Malvasía cabeciblanca</t>
+  </si>
+  <si>
+    <t>Oxyura leucocephala (Scopoli, 1769)</t>
+  </si>
+  <si>
+    <t>Anátida de pequeño tamaño, con el pico ensanchado en su base, cabeza grande, cuerpo compacto y cola relativamente larga. Alas cortas y puntiagudas. O. leucocephala tiene mayor tamaño y la cola más larga que la especie invasora malvasía canela, O. jamaicensis. El perfil del pico es convexo en O. leucocephala, mientras que en O. jamaicensis es cóncavo. O. leucocephala tiene mayor extensión de blanco en la cabeza en machos que los de O. jamaicensis. Las cobertoras inferiores de la cola son grisáceas en O. leucocephala y blancas en O. jamaicensis.
+Hay dos fases de coloración en machos. Los machos en fase clara tienen la cabeza blanca con una mancha negra en la parte superior. Cuello pardo negruzco, pecho castaño y dorso pardo castaño o canela. La parte inferior del pecho es gris plateada y el vientre moteado de pardo. Las alas son pardo grisáceas dorsalmente y ventralmente gris plateado con axilares blancuzcas. La cola es negruzca. Las patas son de color gris azulado. El macho se caracteriza por tener el pico de color azul brillante durante la época de reproducción y gris en otoño e invierno. La extensión de la coloración negra de la parte superior de la cabeza varía entre machos, siendo subadultos los machos con la cabeza negra. Los machos en fase oscura tienen el vientre pardo más oscuro, las plumas cobertoras de la parte inferior de la cola más oscuras y las cobertoras inferiores de las alas más oscuras.
+También hay dos fases de coloración en hembras. Las hembras en fase clara tienen una mancha negra en la parte superior de la cabeza más extensa que en el macho. Por debajo de ésta hay una estrecha banda clara que desde el pico y por debajo del ojo se extiende hacia atrás y por debajo una banda similar de color negruzco. La parte inferior de la cabeza y el cuello es de color blanco grisáceo. La parte superior del pecho es de color pardo rojizo. El resto del cuerpo es como en el macho pero más gris pardo con un barreado más marcado. El pico presenta coloración gris todo el año. En hembras con plumaje oscuro, la coronilla, parte posterior del cuello y banda oscura de los lados de la cabeza de color pardo oscuro, con la punta de las plumas de color castaño.
+Masa corporal media, 717 g en machos y 657 g en hembras.</t>
+  </si>
+  <si>
+    <t>Martinete común</t>
+  </si>
+  <si>
+    <t>Nycticorax nycticorax (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Garza de mediano tamaño (58-66 cm de longitud) inconfundible por su aspecto rechoncho, cuello y patas relativamente cortos y su vuelo distintivo con alas rechonchas y redondas, con dedos que sobresalen poco de la cola. Su plumaje adulto es fácilmente identificable por su parte superior de la cabeza, espalda y escapulares negras, alas, obispillo y cola grises, partes inferiores blancas. Además, tiene el pico negro muy robusto, patas amarillas o verdosas la mayor parte del año que pasan a ser anaranjadas o rosas en época reproductora y ojos rojos.  Los juveniles poseen un plumaje de fondo marrón manchado y veteado de gris, beige y blanquecino, con ojos, patas y pico de color amarillo sucio.
+Masa corporal media, 682 g en machos y 590 g en hembras.</t>
+  </si>
+  <si>
+    <t>Milano negro</t>
+  </si>
+  <si>
+    <t>Milvus migrans (Boddaert, 1783)</t>
+  </si>
+  <si>
+    <t>Rapaz de tamaño medio, con una distintiva silueta de vuelo estilizada y de alas más bien largas y agudas, que en la Península Ibérica sólo ofrece confusión con su congénere el milano real. La cola presenta una escotadura diagnóstica, siendo en el milano negro menos acusada que en el milano real. La coloración del cuerpo es marrón oscuro con la cabeza y el cuello más claros.
+Masa corporal media, 796 g en machos y 914 g en hembras.</t>
+  </si>
+  <si>
+    <t>Mirlo acuático</t>
+  </si>
+  <si>
+    <t>Cinclus cinclus (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Ave de unos 18 cm de tamaño, con cuerpo fusiforme, alas y cola relativamente cortas. Es de color pardo oscuro, con cabeza y nuca marrón, mentón, garganta y pecho de un conspicuo color blanco. Abdomen de color castaño-rojizo o pardo oscuro. Juveniles de color gris pizarra en el dorso, con la parte inferior del cuerpo blanquecina, barrada en el pecho y blanca en mentón y garganta. No existe dimorfismo sexual apreciable en el plumaje.
+Masa corporal media, 65 g en machos y 55 g en hembras.</t>
+  </si>
+  <si>
+    <t>Mirlo capiblanco</t>
+  </si>
+  <si>
+    <t>Turdus torquatus Linnaeus, 1758</t>
+  </si>
+  <si>
+    <t>El macho es negro, a excepción del creciente pectoral blanco; presenta una escamación grisácea o blancuzca sobre el manto, escapulares, pecho y flancos, y bordes blanco grisáceos de las plumas de vuelo y cobertoras alares. Pico amarillo y patas y pies parduscos. La hembra es más parda en cabeza, garganta y escapulares, con pequeño creciente pectoral blancuzco. Joven parecido a la hembra, con estrías beige por encima y garganta blancuzca, sin creciente pectoral.</t>
+  </si>
+  <si>
+    <t>Mirlo común</t>
+  </si>
+  <si>
+    <t>Turdus merula Linnaeus, 1758</t>
+  </si>
+  <si>
+    <t>Zorzal de tamaño mediano a grande de alas redondeadas y cola larga, típicas de ave forestal. 24-29 cm de longitud total. Evidente dimorfismo sexual en plumaje, apreciable en el campo. El macho negro, con pico y anillo ocular amarillos y la hembra parda con pico y anillo ocular poco contrastados. Los juveniles, muy moteados, también son identificables en el campo.
+Masa corporal, 72-123 g.</t>
+  </si>
+  <si>
+    <t>Morito común</t>
+  </si>
+  <si>
+    <t>Plegadis falcinellus (Linnaeus, 1766)</t>
+  </si>
+  <si>
+    <t>El morito común es un tipo de ibis con plumaje marrón con iridiscencias que puede parecer negro desde lejos. Tiene la morfología típica del ibis: cuerpo mediano (tamaño medio: 500-800 g) alargado y de forma ovoide, cuello largo que mantiene estirado en vuelo, alas largas, anchas y apuntadas, cola corta y patas de color marrón oscuro moderadamente largas y que en vuelo sobresalen por detrás de la cola con dedos largos ligeramente palmeados en la base). El pico, muy distintivo, es largo, delgado, acanalado, curvado cóncavamente (i.e. hacia abajo) y de color gris o parduzco. El iris es de color marrón oscuro. En la época de reproducción el plumaje adquiere colores iridiscentes de color bronce, violáceo y verdoso brillantes. No presenta dimorfismo sexual en el plumaje, pero los machos son ligeramente más grandes que las hembras. Los inmaduros se parecen a adultos no reproductores, con un brillo verde aceitoso en la cabeza y el cuello, y una cantidad variable de blanco en la frente, la garganta y el cuello.</t>
+  </si>
+  <si>
+    <t>Mosquitero musical</t>
+  </si>
+  <si>
+    <t>Phylloscopus trochilus (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El mosquitero musical es un pequeño sílvido de 10-12 cm de longitud y de complexión más bien esbelta, con patas finas y pico puntiagudo. Su rasgo más distintivo lo constituye la lista superciliar blancuzca o amarillenta, moderadamente marcada. Su aspecto general es verde pardo grisáceo por encima, a veces algo más pálido y de un verde más brillante en el obispillo. Por debajo es blanco amarillento en garganta y pecho y más blanco en el vientre, si bien en otoño todas las partes inferiores son muy amarillas, sobre todo en las aves de primer año. Patas generalmente rosa pardusco. Carece de bandas alares y de conspicuos márgenes pálidos en las terciarias.
+En mano el mejor criterio discriminativo se basa en la fórmula alar, ya que no presenta la 6ª primaria emarginada. Asimismo, las alas aparecen apuntadas, puesto que la 2ª primaria es más larga que la 6ª.
+No presenta dimorfismo sexual en cuanto al plumaje, pero sí respecto al tamaño, siendo los machos mayores que las hembras. Los jóvenes del año son muy semejantes a los adultos, pero pueden reconocerse en otoño por sus partes inferiores muy amarillas.
+El mosquitero musical es muy parecido a otros mosquiteros, especialmente a los mosquiteros común e ibérico. A primera vista también existe riesgo de confusión con los zarceros y, más improbablemente, con los carriceros o la curruca mosquitera. </t>
+  </si>
+  <si>
+    <t>Paíño europeo</t>
+  </si>
+  <si>
+    <t>Hydrobates pelagicus (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es la más pequeña de las aves marinas europeas. Tiene un tamaño medio de 14-18 cm y un peso medio de 28 gramos. Su plumaje es negro con una mancha blanca en el obispillo y franjas blancas en la cara inferior de las alas. Sus ojos, pico y patas son oscuros. Destacan sus grandes narinas.  Ambos sexos son muy poco dimórficos aunque las hembras presentan un tamaño ligeramente superior. La subespecie atlántica es de menor tamaño que la mediterránea. Vuelan muy próximos a la superficie del mar con planeos y rápidos aleteos. La especie presenta un fuerte olor.
+ </t>
+  </si>
+  <si>
+    <t>Paloma torcaz</t>
+  </si>
+  <si>
+    <t>Columba palumbus Linnaeus, 1758</t>
+  </si>
+  <si>
+    <t>Paloma de tamaño grande, azul grisácea, con marcas blancas en las alas en forma de crecientes y laterales del cuello. Larga cola azulada terminada en banda oscura. Lados del cuello purpúreos y pecho vináceo. Patas y pies rosa. Iris amarillo.
+Masa corporal, 420-613 g.</t>
+  </si>
+  <si>
+    <t>Papamoscas cerrojillo</t>
+  </si>
+  <si>
+    <t>Ficedula hypoleuca (Pallas, 1764)</t>
+  </si>
+  <si>
+    <t>Ave de pequeño tamaño, ligeramente menor que un gorrión común. Cuerpo compacto, cabeza ancha y pico fino. Los ojos, las patas y el pico son negros. En primavera, el plumaje de los machos es un contraste de blanco y negro con una mancha blanca en la frente, mientras que las hembras son de color pardo-grisáceo en el dorso y blanco en la parte inferior. Algunas hembras también presentan mancha blanca. En invierno, los machos son muy parecidos a las hembras.
+Masa corporal media, 12,2 g en machos y 12,5 g en hembras</t>
+  </si>
+  <si>
+    <t>Pardela balear</t>
+  </si>
+  <si>
+    <t>Puffinus mauretanicus Lowe, 1921</t>
+  </si>
+  <si>
+    <t>Ave marina de tamaño medio. La cabeza es pequeña en comparación con el resto del cuerpo. Son específicos de la pardela balear la coloración del plumaje, más oscura en sus partes ventrales, y con un contraste menor con el dorso oscuro que la pardela mediterránea Puffinus yelkouan. Las patas y el pico, como en todo el género Puffinus, son de color oscuro.
+Las alas y cola son cortas. Los machos son en promedio un 5% mayores que las hembras. El vuelo típico de la pardela se realiza a ras de agua, en series de aleteos rápidos entremezclados con planeos.
+Masa corporal media, 495 g.</t>
+  </si>
+  <si>
+    <t>Pardela cenicienta atlántica</t>
+  </si>
+  <si>
+    <t>Calonectris borealis (Cory, 1881)</t>
+  </si>
+  <si>
+    <t>Ave marina con alas largas y delgadas, tiene una envergadura media de 126 cm. Vuela a escasa altura sobre el agua, en largas secuencias de planeo combinadas con secuencias de vuelo activo batiendo las alas.
+C. borealis es en promedio mayor en masa corporal que C. diomedea y su pico es más robusto. El cuello muestra menos contraste con la cabeza y el dorso en borealis, dando la sensación de ser más estrecho que en diomedea. El plumaje de C. borealis se muestra en general más oscuro y contrastado, en particular las partes inferiores, donde el reborde oscuro de las alas se adentra más hacia el interior y define un margen mucho más resaltado que en C. diomedea. En C. borealis, el área blanca de la zona inferior de las alas se restringe a las plumas cobertoras, dando una forma redondeada a dicho área. Por el contrario, en C. diomedea la zona proximal de las primarias más externas es casi blanca, lo que crea un efecto de panel blanco angulado en forma de cuña, no sólo formado por la cobertoras, como en C. borealis, sino también por las primarias.
+Masa corporal media, 785 g.</t>
+  </si>
+  <si>
+    <t>Pardela cenicienta mediterránea</t>
+  </si>
+  <si>
+    <t>Calonectris diomedea (Scopoli, 1769)</t>
+  </si>
+  <si>
+    <t>Ave marina con alas largas y delgadas, tiene una envergadura media de 122 cm. Vuela a escasa altura sobre el agua, en largas secuencias de planeo combinadas con secuencias de vuelo activo batiendo las alas.
+C. diomedea tiene menor tamaño que C. borealis. Su pico es menos robusto y su cuello muestra más contraste con la cabeza y el dorso respecto a la especie atlántica. El plumaje de C. diomedea es algo más claro y menos contrastado que en C. borealis, y sus partes inferiores no muestran un reborde tan resaltado como en aquella. En C. diomedea, la zona proximal de las primarias más externas es casi blanca, lo que crea un efecto de panel blanco angulado en la zona inferior de las alas, no sólo formado por la cobertoras, como en C. borealis, sino también por las primarias.
+Masa corporal media, 647g.</t>
+  </si>
+  <si>
+    <t>Pato colorado</t>
+  </si>
+  <si>
+    <t>Netta rufina (Pallas, 1773)</t>
+  </si>
+  <si>
+    <t>Es un pato buceador grande y robusto, con una amplia franja blanca en las alas de ambos sexos. Es uno de los patos de mayor tamaño entre los que habitualmente se pueden observar en España. Presenta dimorfismo sexual, tanto en coloración del plumaje como en tamaño. Los machos son de mayor tamaño que las hembras en todas las medidas corporales. Los machos pesan 1100 g y las hembras 960 g.
+El macho en plumaje nupcial tiene la cabeza y parte anterior del cuello de color castaño-anaranjado, con el píleo ocre-amarillento. Nuca, pecho, una franja central en el vientre, parte posterior del vientre y obispillo son de color negro lustroso. Los flancos son blancos. Dorso y cobertoras alares son de color marrón-grisáceo. Pico e iris son rojos, en tanto que las patas son rojizas. En plumaje de eclipse es similar a la hembra, pero mantiene pico e iris rojos.
+La hembra tiene la parte superior de la cabeza y parte trasera del cuello de coloración parda, mientras que la parte inferior de la cabeza, del ojo al cuello, y la anterior del cuello son blancuzcas. El resto del cuerpo es de tonalidades pardas, más claras en el vientre. Presenta un plumaje similar todo el año. El pico es negruzco y el iris castaño.
+El plumaje juvenil es similar al de la hembra adulta, pero más oscuro. El pico es negruzco.</t>
+  </si>
+  <si>
+    <t>Perdiz pardilla </t>
+  </si>
+  <si>
+    <t>Perdix perdix (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Perdiz caracterizada por tener una longitud entre 29 y 31 cm y el color ladrillo pálido de garganta y frente y, al volar, por la tonalidad rojiza de las plumas laterales de la cola. Cuello y partes inferiores grises. Partes superiores listadas de color ocráceo  y flancos barreados en castaño. El macho tiene conspicua herradura de color castaño en el bajo pecho (vestigios de la marca, en la hembra) y visible mota roja desnuda detrás del ojo. Patas grises. Joven pardo grisáceo con líneas blancuzcas en el pecho y cabeza parda oscura.
+Masa corporal, 310-455 g.</t>
+  </si>
+  <si>
+    <t>Picamaderos negro</t>
+  </si>
+  <si>
+    <t>Dryocopus martius (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Pájaro carpintero de gran tamaño (46 cm de longitud) y plumaje negro. El píleo es rojo en el macho y solo el cogote en la hembra. Pico blanco hueso. Pies y patas grises.
+Masa corporal: 260-340 g.</t>
+  </si>
+  <si>
+    <t>Pico mediano</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dendropicos medius (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Es un pájaro carpintero de tamaño medio con el píleo rojo que llega desde la frente hasta la nuca. Bigotera poco aparente e incompleta. Cuello y resto de la cara blanco. Espalda negra que se une con el rojo del píleo. Las escapulares forman una mancha blanca y oval. Pecho de coloración amarillenta con listas negras, que se vuelve rosado hacia el vientre y rosa fuerte en la cloaca y las infracoberteras caudales. Escaso dimorfismo sexual en adultos. Juveniles algo más apagados y con el píleo y las áreas rosadas más reducidas.
+Masa corporal media: 55,8 g en machos y 52 g en hembras.  </t>
+  </si>
+  <si>
+    <t>Polluela chica</t>
+  </si>
+  <si>
+    <t>Zapornia pusilla Pallas, 1776</t>
+  </si>
+  <si>
+    <t>Se caracteriza por su pequeño tamaño y patas desarrolladas con dedos muy largos, plumaje con contraste entre las partes superiores, de color marrón y negro con motas irregulares blancas, e inferiores, siendo éstas de color aproximadamente uniforme, gris plomizo cuando son adultas, y con un barreado negro y blanco que abarca el vientre desde más arriba de la inserción de las patas.
+Las hembras tienen el plumaje más pálido y una mayor extensión de blanco en la garganta y vientre que los machos. Este plumaje resulta bastante parecido al de los jóvenes tras la muda postjuvenil.
+Longitud total, 17-19 cm; masa corporal media, 42 g.</t>
+  </si>
+  <si>
+    <t>Porrón pardo</t>
+  </si>
+  <si>
+    <t>Aythya nyroca (Güldenstädt, 1770)</t>
+  </si>
+  <si>
+    <t>Es un pato buceador de tamaño mediano, con una franja blanca en las alas, muy visible en vuelo. Cuando nada o está descansando, la cola queda ligeramente sobre la superficie del agua, más o menos paralela a esta última. Posee la frente plana y una coronilla prominente. Presenta dimorfismo sexual, tanto en coloración del plumaje y del iris como en la longitud del pico.
+El macho en plumaje nupcial presenta cabeza, cuello, pecho, flancos y partes superiores de color pardo rojizo, siendo la coloración más oscura en la base del cuello y partes superiores. Junto a la base de la mandíbula inferior presenta una pequeña mancha de plumaje blanco. El iris es blanco.
+El plumaje nupcial de la hembra es similar al del macho, pero más apagado y de tonalidad menos rojiza. Carece de la pequeña mancha blanca que los machos tienen junto a la base de la mandíbula inferior El iris de las hembras es pardo.
+Los juveniles son parecidos a las hembras adultas, pero con el plumaje de cabeza y cuello de tonalidad más apagada. El iris es más grisáceo que el de las hembras adultas.</t>
+  </si>
+  <si>
+    <t>Quebrantahuesos</t>
+  </si>
+  <si>
+    <t>Gypaetus barbatus (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Tamaño grande, con envergadura media de 2,54 m y la longitud 1,09 m. La silueta en vuelo es esbelta y estilizada, alas estrechas y cola larga.
+En adultos, la coloración de la cabeza, tarsos y región ventral varían del blanco a tonalidades anaranjadas. La parte superior de las plumas que recubren el cuerpo es negro-ceniza. Los ojos, con un iris que varía entre el color marfil y tonalidades amarillentas están rodeados de un anillo esclerótico muy conspicuo. Un antifaz negro se extiende desde los ojos hasta la base del pico donde aparece la barba que se extiende bajo el pico. En la parte superior de la cabeza aparece una mancha de plumas negras que conforman el denominado capirote. Su diseño es muy variable. En la región auricular también se extiende una mancha negra de filoplumas ausente en la subespecie G. b. meridionalis.
+El plumaje varía con la edad, no alcanzándose el plumaje de adulto perfecto hasta los 7 años de vida. El juvenil de primer año tiene la cabeza y cuello negro, iris oscuro y barba muy pequeña. Parte superior de la espalda con un escudo blanco en forma de V. Espalda marrón, cobertoras marrones, ocasionalmente salpicadas de plumas blancas. Plumaje del pecho, vientre y calzas marrones, moteados de claro.
+Masa corporal media, 5,18 kg en machos y 5,85 kg en hembras.</t>
+  </si>
+  <si>
+    <t>Rabilargo</t>
+  </si>
+  <si>
+    <t>Cyanopica cooki Bonaparte, 1850</t>
+  </si>
+  <si>
+    <t>Córvido de pequeño tamaño y de silueta muy parecida a la de la Urraca, con alas y cola de color celeste, cabeza con capirote negro, garganta blanca y dorso y vientre de color gris pardusco. No existen diferencias de coloración entre sexos. Sin embargo, se aprecian diferencias biométricas entre sexos y clases de edad en determinadas variables. Los adultos son algo mayores que los jóvenes y los machos mayores que las hembras. Los adultos realizan muda completa a finales de la primavera y los juveniles muda parcial en verano. Dimorfismo sexual en la extensión de la muda postjuvenil.
+Masa corporal media, 70 g.</t>
+  </si>
+  <si>
+    <t>Reyezuelo listado</t>
+  </si>
+  <si>
+    <t>Regulus ignicapilla (Temminck, 1820)</t>
+  </si>
+  <si>
+    <t>Ave de pequeño tamaño, con 9 cm de longitud. Ceja blanca y lista ocular negra muy patentes. El macho adulto presenta el píleo anaranjado y de gran tamaño, mientras en el caso de la hembra es menor y más bien amarillento. El dorso es de color verde oliváceo, mientras las partes inferiores son blanquecinas.
+Masa corporal, 5-6g.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roquero solitario </t>
+  </si>
+  <si>
+    <t>Monticola solitarius (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>El macho adulto tiene el plumaje de color azul, excepto las alas y la cola que son de color pizarroso oscuro. La hembra es de color pardo oscuro, con el pecho y cuello con manchas claras bordeadas de pardo rojizo y el dorso gris azulado. Vientre rayado con líneas pardo-rojizas orilladas de blanco sucio.
+En el macho adulto el pico es negro grisáceo y en la hembra adulta negro parduzco. Las patas en adultos son de color negro, negro grisáceo o de color cuerno parduzco.
+Longitud total, 230 mm. Masa corporal, 47-70,5 g.</t>
+  </si>
+  <si>
+    <t>Ruiseñor común</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Luscinia megarhynchos (Brehm, 1831)</t>
+  </si>
+  <si>
+    <t>Paseriforme de tamaño medio, con plumaje pardo por encima y blanco sucio por debajo, pecho y flancos ligeramente ocres. La zona inferior (garganta, pecho y vientre) presenta coloración más clara con plumas blanco amarillento. Las alas son pardas, aunque ligeramente más pálidas que el dorso. Se trata de un ave con una figura estilizada y cola larga y ancha, con plumas de color rojizo. Sin dimorfismo sexual en plumaje.</t>
+  </si>
+  <si>
+    <t>Ruiseñor pechiazul </t>
+  </si>
+  <si>
+    <t>Luscinia svecica (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Paseriforme de 14 cm de longitud, que muestra un plumaje con un claro dimorfismo sexual. En machos, mentón y garganta azul metálico con medallón blanco en el centro (aunque en España el babero es totalmente azul en muchos machos), seguidos hacia la parte ventral por una banda estrecha negra, otra blanca que no existe en las poblaciones reproductoras ibéricas y otra mayor de color rojo. En plumaje no nupcial, el babero azul casi desaparece. La hembra carece de babero azul y presenta un collar de puntos negros, ocasionalmente manchado de puntos azules. Muda parcial en jóvenes y completa en adultos tras periodo de cría. Además, muda prenupcial, parcial, especialmente en machos.
+Masa corporal, 12 g.</t>
+  </si>
+  <si>
+    <t>Sisón común</t>
+  </si>
+  <si>
+    <t>Tetrax tetrax (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Es un ave de mediano tamaño que mide 40-45 cm y tiene una envergadura de 105-115 cm. El macho en plumaje nupcial tiene el píleo y dorso ocre vermiculado y un llamativo cuello negro con un collar blanco en forma de uve. La hembra es de color pardo arenoso con un fino vermiculado negro en el píleo, cuello, dorso y parte superior del pecho. Los jóvenes se parecen a las hembras. En invierno, macho, hembra y joven presentan un plumaje ocre vermiculado que los hace indistinguibles salvo por el tamaño. La emarginación de la séptima primaria en los machos produce un siseo característico en vuelo.
+Masa corporal, 740-910 g en machos y 700 y 750 g en hembras.</t>
+  </si>
+  <si>
+    <t>Tarabilla canaria</t>
+  </si>
+  <si>
+    <t>Saxicola dacotiae (Meade-Waldo, 1889)</t>
+  </si>
+  <si>
+    <t>15 cm de envergadura y 11 cm de altura. Los machos presentan un color pardusco por el dorso y pecho blancuzco, aunque exhiben un parche, de extensión muy variable entre individuos, de color naranja debajo de la garganta. La cabeza es negra como en la tarabilla común, pero difiere de ésta por tener la garganta blanca, y también por mostrar una conspicua ceja superciliar blanca (muy variable también en extensión). La hembra tiene el dorso y cabeza pardusca y, al igual que los machos, presentan la ceja superciliar blanca y coloración naranja en el pecho, pero ambas características son significativamente menos extensas.
+Masa corporal, 10,9-13,7 g.</t>
+  </si>
+  <si>
+    <t>Tarabilla norteña</t>
+  </si>
+  <si>
+    <t>Saxicola rubetra (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Ave pequeña (12 cm), de talla similar a la Tarabilla común pero de aspecto un poco menos compacto y redondeado, que se posa erguida y sacude o hace vibrar la cola. Partes superiores pardo-amarillentas moteadas de oscuro, incluido el obispillo. Lados de la cabeza oscuros y garganta y pecho pardo-anaranjados. Tienen una conspicua lista superciliar de color blanca o crema, alas pardas con marcas alares blancas y cola oscura flanqueada por rectrices externas blancas en su base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarabilla europea </t>
+  </si>
+  <si>
+    <t>Saxicola rubicola (Linnaeus, 1766)</t>
+  </si>
+  <si>
+    <t>Paseriforme pequeño de unos 13 cm de longitud y 15 g de peso. El macho presenta la cabeza con colores negros o pardo oscuros, con un collar blanco a ambos lados del cuello. En contra de lo que ocurre con las tarabillas norteña y canaria, la tarabilla europea no tiene una ceja superciliar blanca. El color blanco también está presente en las grandes cobertoras internas. El obispillo es blanco en los machos y castaño en las hembras. El pecho es anaranjado en ambos sexos con una extensión variable, y las patas y pico son de color negro. La hembras y juveniles tienen tonos parduscos con motas negruzcas. Es habitual ver a esta especie posada en lo alto de arbustos, piedras grandes o elementos antrópicos desde donde otea las proximidades en busca de invertebrados.</t>
+  </si>
+  <si>
+    <t>Tarro blanco</t>
+  </si>
+  <si>
+    <t>Tadorna tadorna (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>El tarro blanco es una anátida de tamaño grande, con coloración del plumaje similar en machos y hembras. A distancia su plumaje parece blanco y negro, pero la cabeza es de coloración negro-verdosa, normalmente con blanco en la frente de la hembra. Ésta también puede tener áreas o manchas variables pálidas a ambos lados de la cara, que posibilitan la identificación individual en algunos casos. El plumaje del cuello es negro en su parte superior y blanco en la inferior. El cuerpo es blanco con una banda castaña que cruza el pecho, más ancha e intensamente coloreada en el macho. Las escapulares son negras y hay una franja negra a lo largo del vientre, también más ancha y oscura en los machos. Las infracobertoras caudales son de color canela, más oscuras en el macho que en la hembra. Las cobertoras alares de los adultos son blancas, contrastando con las primarias negras, las secundarias verde iridiscentes, y un grupo de terciarias terminadas en color castaño intenso. La cola es blanca con el extremo negro. Pico rojo brillante con una llamativa protuberancia basal de color rojo en machos.
+Masa corporal, 830-1.500 g en machos y 562-1.250 g en hembras.</t>
+  </si>
+  <si>
+    <t>Tarro canelo</t>
+  </si>
+  <si>
+    <t>Tadorna ferruginea (Pallas, 1764)</t>
+  </si>
+  <si>
+    <t>Pato grande, con el pico pequeño y con coloración corporal pardo-anaranjada y la cabeza más clara. Primarias, secundarias y rectrices de color negro, en fuerte contraste con las coberteras alares que son de color blanco. El pico y las patas son negruzcos. Los machos y las hembras son similares, solamente se diferencian en que los machos tienen un pequeño collar negruzco poco marcado.
+Longitud total, 50-67 cm; envergadura, 121-145 cm. Masa corporal media, 1.331 g.</t>
+  </si>
+  <si>
+    <t>Treparriscos</t>
+  </si>
+  <si>
+    <t>Tichodroma muraria (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>El macho tiene partes superiores grises, supracobertoras alares carmín, y rosa carmín sobre álula y grandes cobertoras. Primarias gris oscuro con carmín en la base de los vexilos externos y puntas negras; hay dos óvalos blancos, uno grande fuera y otro pequeño interno, en las cuatro primeras primarias. Garganta y pecho negro, zonas inferiores gris ceniza y cola negra, con puntas grises, blancuzcas en las rectrices externas. Pico largo, fino y curvado hacia abajo, negro como las patas. La hembra posee garganta y pecho gris blancuzco. Alas anchas y redondeadas, muy conspicuas por las marcas carmín y blanco.
+Masa corporal media: 18,5 g en machos y 18 g en hembras</t>
+  </si>
+  <si>
+    <t>Urogallo común</t>
+  </si>
+  <si>
+    <t>Tetrao urogallus (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Ave galliforme de gran tamaño y con un acusado dimorfismo sexual, tanto en tamaño como en coloración. Los machos son más grandes que un gallo doméstico y las hembras de similar tamaño al de una gallina. Los machos adultos son de colores oscuros, con el cuerpo y la cola de color pizarra y las alas de marrones. Las hembras tienen el dorso de ocre con motas o franjas de color negro, el vientre del mismo color aunque más uniforme y el vientre de color ocre muy claro, casi blanco. En los adultos, ambos sexos tienen el pico de color marfil y ébano y una carúncula roja sobre los ojos, más notoria en los machos.
+Masa corporal: 2,9- 3,8 kg en machos y 1.5-1,7 kg en hembras.</t>
+  </si>
+  <si>
+    <t>Urraca</t>
+  </si>
+  <si>
+    <t>Pica pica Linnaeus, 1758</t>
+  </si>
+  <si>
+    <t>Ave blanca y negra de tamaño mediano, entre 43 y 50 cm incluyendo su cola, negra y bastante larga (20 a 25 cm) y graduada en aspecto, ya que las plumas centrales son las más largas y su tamaño disminuye hacia el exterior.
+Masa corporal media, 201 g en machos y 184 g en hembras.</t>
+  </si>
+  <si>
+    <t>Zarapito real</t>
+  </si>
+  <si>
+    <t>Numenius arquata (Linnaeus, 1758)</t>
+  </si>
+  <si>
+    <t>Zarapito grande, con una longitud de 50-60 cm y envergadura de 80-100 cm. Presenta plumaje nupcial caracterizado por ceja indistinta, lunar oscuro frente al ojo, parte superior marrón negruzco jaspeado de ante; pecho, cuello y flancos superiores teñidos de ante con estrías marcadas y resto de las partes inferiores blancas. Posee pico curvado, siendo el de la hembra mayor que el del macho.
+Masa corporal, 540-1000 g en machos y 700-1300 g en hembras.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zorzal charlo </t>
+  </si>
+  <si>
+    <t>Turdus viscivorus Linnaeus, 1758</t>
+  </si>
+  <si>
+    <t>Zorzal grande, con partes superiores pardo-grisáceas y partes inferiores blancuzcas con numerosas motas oscuras de disposición irregular; rectrices externas con puntas blancas distintivas; infracoberteras alares blancas, muy visibles en vuelo. Sexos similares. Jóvenes con manchas blancas y ocres en las partes superiores.
+Masa corporal: 96-134 g en machos y 106-140 g en hembras; longitud: 26-28 cm; envergadura: 42-47 cm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zorzal común </t>
+  </si>
+  <si>
+    <t>Turdus philomelos C. L. Brehm, 1831</t>
+  </si>
+  <si>
+    <t>La coloración es parda por encima, obispillo con tinte aceitunado, débil presencia de manchas crema en las cobertoras alares, barra auricular oscura vaga y tonos blancuzcos por debajo con tintes cremosos en los flancos. Moteado oscuro regular en pecho, vientre y flancos. Infracobertoras alares amarillentas, muy visibles en vuelo. Pico oscuro, de base pálida, y pies y patas rosadas. Iris avellana. Sexos similares.
+Masa corporal, 42-107 g.</t>
+  </si>
+  <si>
+    <r>
+      <t>Merops apiaster</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> Linnaeus, 1758</t>
+    </r>
+  </si>
+  <si>
+    <t>VertebradosIbericos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -836,6 +1478,11 @@
       <i/>
       <sz val="8"/>
       <color rgb="FFC0C0C0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -868,9 +1515,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1151,11 +1796,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1182,830 +1827,1782 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3" t="s">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="C33" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3" t="s">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="C40" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3" t="s">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3" t="s">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="C43" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="C44" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="C45" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C46" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="C48" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="C49" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C50" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3" t="s">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="C51" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3" t="s">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="C52" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3" t="s">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="C53" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3" t="s">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="C54" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3" t="s">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="C55" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3" t="s">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="C56" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3" t="s">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="C58" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C61" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3" t="s">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="3" t="s">
+      <c r="B62" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="C62" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D62" s="3" t="s">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" s="3" t="s">
+      <c r="B63" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="C63" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D63" s="3" t="s">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="2" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" s="3" t="s">
+      <c r="B64" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="C64" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D64" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D64" s="3" t="s">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="C65" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D65" s="3" t="s">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="C66" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D66" s="3" t="s">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="3" t="s">
+      <c r="B67" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="C67" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D67" s="3" t="s">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="3" t="s">
+      <c r="B68" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="C68" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D68" s="3" t="s">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" s="3" t="s">
+      <c r="B69" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="C69" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D69" s="3" t="s">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="B70" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="A71" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="A72" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="A73" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A98" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A99" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A100" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A101" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A102" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A103" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A104" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A105" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A106" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A107" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A108" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A109" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A110" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A111" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A112" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A115" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A116" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A117" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A118" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A119" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A120" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A121" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A122" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A123" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A124" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A125" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A126" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A127" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A128" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>383</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>